<commit_message>
adding anitha's code and login nonemsuser code
</commit_message>
<xml_diff>
--- a/resources/TestData/LoginPage.xlsx
+++ b/resources/TestData/LoginPage.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="invalidLoginCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="nonExistingEMSUser" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>test data</t>
   </si>
@@ -376,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,6 +403,49 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>